<commit_message>
Tried to improve font situation...
</commit_message>
<xml_diff>
--- a/_data/workshops.xlsx
+++ b/_data/workshops.xlsx
@@ -1761,7 +1761,7 @@
   <dimension ref="A1:BF36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="2" spans="1:58">
       <c r="A2">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>271</v>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="3" spans="1:58">
       <c r="A3">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>301</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="4" spans="1:58">
       <c r="A4">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>336</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="5" spans="1:58">
       <c r="A5">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>168</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="6" spans="1:58">
       <c r="A6">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>94</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="7" spans="1:58">
       <c r="A7">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>256</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="8" spans="1:58">
       <c r="A8">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>64</v>
@@ -2359,7 +2359,7 @@
     </row>
     <row r="9" spans="1:58">
       <c r="A9">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>132</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="10" spans="1:58">
       <c r="A10">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>196</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="11" spans="1:58">
       <c r="A11">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>249</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="12" spans="1:58">
       <c r="A12">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>152</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="13" spans="1:58">
       <c r="A13">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>239</v>

</xml_diff>